<commit_message>
Finished final edits of main text, still need to fill in performance stats
</commit_message>
<xml_diff>
--- a/manuscript/figures/xpresspipe_supplement1.xlsx
+++ b/manuscript/figures/xpresspipe_supplement1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordan/Desktop/xpressyourself_manuscript/manuscript/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222649F5-85CB-D849-9C0E-86BB0DFB5227}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041D6E0B-9383-0B49-8F77-899DF4E031F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13580" yWindow="1460" windowWidth="30800" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Isoform quantification</t>
   </si>
   <si>
-    <t>Differential Expression Analysis</t>
-  </si>
-  <si>
     <t xml:space="preserve">Read size distribution </t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t xml:space="preserve">General quality control </t>
   </si>
   <si>
-    <t>rRNA probe summary</t>
-  </si>
-  <si>
     <t>Other customizable analyses</t>
   </si>
   <si>
@@ -220,6 +214,12 @@
   </si>
   <si>
     <t>Translation efficiency calculation and analysis</t>
+  </si>
+  <si>
+    <t>rRNA probe summary and design</t>
+  </si>
+  <si>
+    <t>Differential expression analysis</t>
   </si>
 </sst>
 </file>
@@ -279,7 +279,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -387,11 +387,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -429,13 +442,14 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="30"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="30"/>
     </xf>
@@ -448,13 +462,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="30"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,114 +825,114 @@
     <row r="1" spans="2:45" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:45" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="2:45" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C3" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="29"/>
+        <v>35</v>
+      </c>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="2:45" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="12"/>
     </row>
     <row r="5" spans="2:45" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="31"/>
+        <v>42</v>
+      </c>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="2:45" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="15"/>
-      <c r="D6" s="32"/>
+      <c r="D6" s="26"/>
     </row>
     <row r="7" spans="2:45" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="M7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="2" t="s">
+      <c r="X7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y7" s="2" t="s">
+      <c r="Z7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Z7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="AC7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:45" ht="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -954,7 +964,7 @@
     <row r="9" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>
       <c r="C9" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -979,14 +989,14 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="7"/>
-      <c r="AA9" s="29"/>
+      <c r="AA9" s="23"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
       <c r="AD9" s="7"/>
     </row>
     <row r="10" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>53</v>
+      <c r="B10" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>0</v>
@@ -1020,9 +1030,9 @@
       <c r="AD10" s="4"/>
     </row>
     <row r="11" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1053,9 +1063,9 @@
       <c r="AD11" s="4"/>
     </row>
     <row r="12" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1086,14 +1096,14 @@
       <c r="AD12" s="6"/>
     </row>
     <row r="13" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="25" t="s">
-        <v>54</v>
+      <c r="B13" s="28" t="s">
+        <v>52</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="29"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="10"/>
       <c r="G13" s="4"/>
       <c r="H13" s="7"/>
@@ -1121,9 +1131,9 @@
       <c r="AD13" s="7"/>
     </row>
     <row r="14" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="27"/>
+      <c r="B14" s="30"/>
       <c r="C14" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="7"/>
@@ -1154,8 +1164,8 @@
       <c r="AD14" s="7"/>
     </row>
     <row r="15" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
-        <v>55</v>
+      <c r="B15" s="28" t="s">
+        <v>53</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>1</v>
@@ -1189,7 +1199,7 @@
       <c r="AD15" s="7"/>
     </row>
     <row r="16" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="13" t="s">
         <v>2</v>
       </c>
@@ -1220,21 +1230,21 @@
       <c r="AB16" s="7"/>
       <c r="AC16" s="7"/>
       <c r="AD16" s="7"/>
-      <c r="AG16" s="23"/>
-      <c r="AI16" s="23"/>
-      <c r="AJ16" s="23"/>
-      <c r="AK16" s="23"/>
-      <c r="AL16" s="23"/>
-      <c r="AM16" s="23"/>
-      <c r="AN16" s="23"/>
-      <c r="AO16" s="23"/>
-      <c r="AP16" s="23"/>
-      <c r="AQ16" s="23"/>
-      <c r="AR16" s="23"/>
-      <c r="AS16" s="23"/>
+      <c r="AG16" s="21"/>
+      <c r="AI16" s="21"/>
+      <c r="AJ16" s="21"/>
+      <c r="AK16" s="21"/>
+      <c r="AL16" s="21"/>
+      <c r="AM16" s="21"/>
+      <c r="AN16" s="21"/>
+      <c r="AO16" s="21"/>
+      <c r="AP16" s="21"/>
+      <c r="AQ16" s="21"/>
+      <c r="AR16" s="21"/>
+      <c r="AS16" s="21"/>
     </row>
     <row r="17" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="19" t="s">
         <v>3</v>
       </c>
@@ -1265,22 +1275,22 @@
       <c r="AB17" s="7"/>
       <c r="AC17" s="7"/>
       <c r="AD17" s="7"/>
-      <c r="AG17" s="23"/>
-      <c r="AI17" s="23"/>
-      <c r="AJ17" s="23"/>
-      <c r="AK17" s="23"/>
-      <c r="AL17" s="23"/>
-      <c r="AM17" s="23"/>
-      <c r="AN17" s="23"/>
-      <c r="AO17" s="23"/>
-      <c r="AP17" s="23"/>
-      <c r="AQ17" s="23"/>
-      <c r="AR17" s="23"/>
-      <c r="AS17" s="23"/>
+      <c r="AG17" s="21"/>
+      <c r="AI17" s="21"/>
+      <c r="AJ17" s="21"/>
+      <c r="AK17" s="21"/>
+      <c r="AL17" s="21"/>
+      <c r="AM17" s="21"/>
+      <c r="AN17" s="21"/>
+      <c r="AO17" s="21"/>
+      <c r="AP17" s="21"/>
+      <c r="AQ17" s="21"/>
+      <c r="AR17" s="21"/>
+      <c r="AS17" s="21"/>
     </row>
     <row r="18" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>56</v>
+      <c r="B18" s="28" t="s">
+        <v>54</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>4</v>
@@ -1326,7 +1336,7 @@
       <c r="AS18" s="15"/>
     </row>
     <row r="19" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="13" t="s">
         <v>5</v>
       </c>
@@ -1371,9 +1381,9 @@
       <c r="AS19" s="15"/>
     </row>
     <row r="20" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="7"/>
@@ -1388,7 +1398,7 @@
       <c r="N20" s="7"/>
       <c r="O20" s="4"/>
       <c r="P20" s="9"/>
-      <c r="Q20" s="30"/>
+      <c r="Q20" s="24"/>
       <c r="R20" s="7"/>
       <c r="S20" s="7"/>
       <c r="T20" s="9"/>
@@ -1404,13 +1414,13 @@
       <c r="AD20" s="7"/>
     </row>
     <row r="21" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D21" s="29"/>
+        <v>60</v>
+      </c>
+      <c r="D21" s="23"/>
       <c r="E21" s="5"/>
-      <c r="F21" s="30"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="4"/>
@@ -1437,16 +1447,16 @@
       <c r="AD21" s="5"/>
     </row>
     <row r="22" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="27"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="19" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="12"/>
       <c r="F22" s="9"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="29"/>
+      <c r="I22" s="23"/>
       <c r="J22" s="7"/>
       <c r="K22" s="4"/>
       <c r="L22" s="7"/>
@@ -1470,13 +1480,13 @@
       <c r="AD22" s="7"/>
     </row>
     <row r="23" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
-        <v>57</v>
+      <c r="B23" s="27" t="s">
+        <v>55</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="29"/>
+        <v>46</v>
+      </c>
+      <c r="D23" s="23"/>
       <c r="E23" s="7"/>
       <c r="F23" s="9"/>
       <c r="G23" s="7"/>
@@ -1505,12 +1515,12 @@
       <c r="AD23" s="7"/>
     </row>
     <row r="24" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="24"/>
+      <c r="B24" s="27"/>
       <c r="C24" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="29"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="11"/>
       <c r="G24" s="7"/>
       <c r="H24" s="4"/>
@@ -1521,28 +1531,28 @@
       <c r="M24" s="4"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
-      <c r="P24" s="30"/>
+      <c r="P24" s="24"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="7"/>
-      <c r="S24" s="29"/>
+      <c r="S24" s="23"/>
       <c r="T24" s="11"/>
       <c r="U24" s="7"/>
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
-      <c r="X24" s="29"/>
+      <c r="X24" s="23"/>
       <c r="Y24" s="4"/>
-      <c r="Z24" s="29"/>
-      <c r="AA24" s="29"/>
+      <c r="Z24" s="23"/>
+      <c r="AA24" s="23"/>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="29"/>
+      <c r="AC24" s="23"/>
       <c r="AD24" s="7"/>
     </row>
     <row r="25" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>58</v>
+      <c r="B25" s="28" t="s">
+        <v>56</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1573,9 +1583,9 @@
       <c r="AD25" s="4"/>
     </row>
     <row r="26" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="24"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1606,9 +1616,9 @@
       <c r="AD26" s="4"/>
     </row>
     <row r="27" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="24"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1639,9 +1649,9 @@
       <c r="AD27" s="5"/>
     </row>
     <row r="28" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="24"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1672,9 +1682,9 @@
       <c r="AD28" s="7"/>
     </row>
     <row r="29" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="24"/>
-      <c r="C29" s="19" t="s">
-        <v>36</v>
+      <c r="B29" s="29"/>
+      <c r="C29" s="31" t="s">
+        <v>34</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
@@ -1698,16 +1708,16 @@
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
-      <c r="Z29" s="29"/>
+      <c r="Z29" s="23"/>
       <c r="AA29" s="7"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="4"/>
     </row>
     <row r="30" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="21" t="s">
-        <v>27</v>
+      <c r="B30" s="30"/>
+      <c r="C30" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="7"/>
@@ -1738,11 +1748,11 @@
       <c r="AD30" s="7"/>
     </row>
     <row r="31" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="24" t="s">
-        <v>59</v>
+      <c r="B31" s="27" t="s">
+        <v>57</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="7"/>
@@ -1773,9 +1783,9 @@
       <c r="AD31" s="7"/>
     </row>
     <row r="32" spans="2:45" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="24"/>
-      <c r="C32" s="28" t="s">
-        <v>60</v>
+      <c r="B32" s="27"/>
+      <c r="C32" s="22" t="s">
+        <v>58</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="12"/>
@@ -1785,9 +1795,9 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="29"/>
+      <c r="L32" s="23"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="29"/>
+      <c r="N32" s="23"/>
       <c r="O32" s="4"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="11"/>
@@ -1806,14 +1816,14 @@
       <c r="AD32" s="4"/>
     </row>
     <row r="33" spans="2:30" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="24"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="29"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -1833,7 +1843,7 @@
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
       <c r="Z33" s="4"/>
-      <c r="AA33" s="29"/>
+      <c r="AA33" s="23"/>
       <c r="AB33" s="7"/>
       <c r="AC33" s="7"/>
       <c r="AD33" s="7"/>
@@ -1989,12 +1999,12 @@
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B25:B29"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B25:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="66" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>